<commit_message>
Finish the reading and writing files in pandas
</commit_message>
<xml_diff>
--- a/data/example1.xlsx
+++ b/data/example1.xlsx
@@ -1,51 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Income</t>
-  </si>
-  <si>
-    <t>Limit</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -60,35 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -376,572 +420,582 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Income</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Limit</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="n">
+        <v>19.225</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>19.225</v>
-      </c>
-      <c r="C2">
-        <v>1433</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>43.54</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>2906</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1">
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>152.298</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>12066</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1">
+    <row r="5">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>55.367</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="n">
         <v>6340</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1">
+    <row r="6">
+      <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n">
         <v>11.741</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="n">
         <v>2271</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1">
+    <row r="7">
+      <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="n">
         <v>15.56</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="n">
         <v>4307</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1">
+    <row r="8">
+      <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="n">
         <v>59.53</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="n">
         <v>7518</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1">
+    <row r="9">
+      <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="n">
         <v>20.191</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="n">
         <v>5767</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1">
+    <row r="10">
+      <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="n">
         <v>48.498</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="n">
         <v>6040</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1">
+    <row r="11">
+      <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="n">
         <v>30.733</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="n">
         <v>2832</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1">
+    <row r="12">
+      <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="n">
         <v>16.479</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="n">
         <v>5435</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1">
+    <row r="13">
+      <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="n">
         <v>38.009</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="n">
         <v>3075</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1">
+    <row r="14">
+      <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="n">
         <v>14.084</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="n">
         <v>855</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1">
+    <row r="15">
+      <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="n">
         <v>14.312</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="n">
         <v>5382</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1">
+    <row r="16">
+      <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="n">
         <v>26.0669999999999</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="n">
         <v>3388</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1">
+    <row r="17">
+      <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="n">
         <v>36.295</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="n">
         <v>2963</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1">
+    <row r="18">
+      <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="n">
         <v>83.851</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="n">
         <v>8494</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1">
+    <row r="19">
+      <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="n">
         <v>21.153</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="n">
         <v>3736</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1">
+    <row r="20">
+      <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="n">
         <v>17.976</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="n">
         <v>2433</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1">
+    <row r="21">
+      <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="n">
         <v>68.71299999999999</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="n">
         <v>7582</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1">
+    <row r="22">
+      <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="n">
         <v>146.183</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="n">
         <v>9540</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1">
+    <row r="23">
+      <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23">
+      <c r="B23" t="n">
         <v>15.8459999999999</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="n">
         <v>4768</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1">
+    <row r="24">
+      <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="n">
         <v>12.0309999999999</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="n">
         <v>3182</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1">
+    <row r="25">
+      <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="n">
         <v>16.819</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="n">
         <v>1337</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="1">
+    <row r="26">
+      <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26">
+      <c r="B26" t="n">
         <v>39.11</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="n">
         <v>3189</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1">
+    <row r="27">
+      <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B27">
+      <c r="B27" t="n">
         <v>107.986</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="n">
         <v>6033</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1">
+    <row r="28">
+      <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B28">
+      <c r="B28" t="n">
         <v>13.561</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="n">
         <v>3261</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="1">
+    <row r="29">
+      <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B29">
+      <c r="B29" t="n">
         <v>34.537</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="n">
         <v>3271</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="1">
+    <row r="30">
+      <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="n">
         <v>28.575</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="n">
         <v>2959</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="1">
+    <row r="31">
+      <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B31">
+      <c r="B31" t="n">
         <v>46.007</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="n">
         <v>6637</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1">
+    <row r="32">
+      <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B32">
+      <c r="B32" t="n">
         <v>69.251</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="n">
         <v>6386</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="1">
+    <row r="33">
+      <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B33">
+      <c r="B33" t="n">
         <v>16.482</v>
       </c>
-      <c r="C33">
+      <c r="C33" t="n">
         <v>3326</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1">
+    <row r="34">
+      <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B34">
+      <c r="B34" t="n">
         <v>40.442</v>
       </c>
-      <c r="C34">
+      <c r="C34" t="n">
         <v>4828</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="1">
+    <row r="35">
+      <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B35">
+      <c r="B35" t="n">
         <v>35.177</v>
       </c>
-      <c r="C35">
+      <c r="C35" t="n">
         <v>2117</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="1">
+    <row r="36">
+      <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B36">
+      <c r="B36" t="n">
         <v>91.36199999999999</v>
       </c>
-      <c r="C36">
+      <c r="C36" t="n">
         <v>9113</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="1">
+    <row r="37">
+      <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B37">
+      <c r="B37" t="n">
         <v>27.039</v>
       </c>
-      <c r="C37">
+      <c r="C37" t="n">
         <v>2161</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1">
+    <row r="38">
+      <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B38">
+      <c r="B38" t="n">
         <v>23.0119999999999</v>
       </c>
-      <c r="C38">
+      <c r="C38" t="n">
         <v>1410</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="1">
+    <row r="39">
+      <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B39">
+      <c r="B39" t="n">
         <v>27.241</v>
       </c>
-      <c r="C39">
+      <c r="C39" t="n">
         <v>1402</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="1">
+    <row r="40">
+      <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B40">
+      <c r="B40" t="n">
         <v>148.08</v>
       </c>
-      <c r="C40">
+      <c r="C40" t="n">
         <v>8157</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="1">
+    <row r="41">
+      <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B41">
+      <c r="B41" t="n">
         <v>62.602</v>
       </c>
-      <c r="C41">
+      <c r="C41" t="n">
         <v>7056</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="1">
+    <row r="42">
+      <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B42">
+      <c r="B42" t="n">
         <v>11.808</v>
       </c>
-      <c r="C42">
+      <c r="C42" t="n">
         <v>1300</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="1">
+    <row r="43">
+      <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B43">
+      <c r="B43" t="n">
         <v>29.564</v>
       </c>
-      <c r="C43">
+      <c r="C43" t="n">
         <v>2529</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="1">
+    <row r="44">
+      <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B44">
+      <c r="B44" t="n">
         <v>27.578</v>
       </c>
-      <c r="C44">
+      <c r="C44" t="n">
         <v>2531</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="1">
+    <row r="45">
+      <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B45">
+      <c r="B45" t="n">
         <v>26.427</v>
       </c>
-      <c r="C45">
+      <c r="C45" t="n">
         <v>5533</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="1">
+    <row r="46">
+      <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B46">
+      <c r="B46" t="n">
         <v>57.202</v>
       </c>
-      <c r="C46">
+      <c r="C46" t="n">
         <v>3411</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="1">
+    <row r="47">
+      <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B47">
+      <c r="B47" t="n">
         <v>123.298999999999</v>
       </c>
-      <c r="C47">
+      <c r="C47" t="n">
         <v>8376</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="1">
+    <row r="48">
+      <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B48">
+      <c r="B48" t="n">
         <v>18.145</v>
       </c>
-      <c r="C48">
+      <c r="C48" t="n">
         <v>3461</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="1">
+    <row r="49">
+      <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B49">
+      <c r="B49" t="n">
         <v>23.793</v>
       </c>
-      <c r="C49">
+      <c r="C49" t="n">
         <v>3821</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="1">
+    <row r="50">
+      <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B50">
+      <c r="B50" t="n">
         <v>10.7259999999999</v>
       </c>
-      <c r="C50">
+      <c r="C50" t="n">
         <v>1568</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="1">
+    <row r="51">
+      <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B51">
+      <c r="B51" t="n">
         <v>23.283</v>
       </c>
-      <c r="C51">
+      <c r="C51" t="n">
         <v>5443</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>